<commit_message>
Made a bunch of comments (labeled COMMENT(Arthur)) and suggestions. Renamed 'Tutorial construction' to 'TutorialConstruction' to enable hierarchical package naming.
add .pdf to .gitignore
</commit_message>
<xml_diff>
--- a/Exercise 1 -- Model building/Model template.xlsx
+++ b/Exercise 1 -- Model building/Model template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="19815" windowHeight="5835" activeTab="4"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="27960" windowHeight="17560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Submodels" sheetId="1" r:id="rId1"/>
@@ -13,21 +13,29 @@
     <sheet name="Reactions" sheetId="4" r:id="rId4"/>
     <sheet name="Parameters" sheetId="5" r:id="rId5"/>
     <sheet name="References" sheetId="6" r:id="rId6"/>
+    <sheet name="Constants" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Compartments!$A$1:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parameters!$A$1:$F$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Reactions!$A$1:$K$177</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">References!$A$1:$E$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$1:$L$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Species!$A$2:$L$148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Submodels!$A$1:$C$5</definedName>
+    <definedName name="Avogadro_constant">Constants!$B$2</definedName>
+    <definedName name="Cell_volume">Constants!$B$3</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -360,6 +368,54 @@
   </si>
   <si>
     <t>Donor horse serum</t>
+  </si>
+  <si>
+    <t>alloliter</t>
+  </si>
+  <si>
+    <t>8 hours</t>
+  </si>
+  <si>
+    <t>take from genes and metabolites; each gene describes an mRNA and a protein; avoid collisions</t>
+  </si>
+  <si>
+    <t>from genes and metabolites</t>
+  </si>
+  <si>
+    <t>also from genes and metabolites</t>
+  </si>
+  <si>
+    <t>metabolite, RNA, or protein</t>
+  </si>
+  <si>
+    <t>RNA or protein seq</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>for some metabolites</t>
+  </si>
+  <si>
+    <t>for prot &amp; RNA, (expression / NA * cell V)</t>
+  </si>
+  <si>
+    <t>Cell volume</t>
+  </si>
+  <si>
+    <t>Avogadro constant (AN)</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>RNA</t>
+  </si>
+  <si>
+    <t>protein</t>
   </si>
 </sst>
 </file>
@@ -369,7 +425,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -397,6 +453,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -421,10 +499,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -450,8 +536,18 @@
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -821,22 +917,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -847,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -858,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -869,7 +965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -880,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -894,30 +990,35 @@
   </sheetData>
   <autoFilter ref="A1:C5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="36">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -944,8 +1045,11 @@
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -962,656 +1066,706 @@
   </sheetData>
   <autoFilter ref="A1:D3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L146"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" zoomScalePageLayoutView="166" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="14.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.28515625" style="3" customWidth="1"/>
-    <col min="10" max="11" width="10.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="21.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.33203125" style="3" customWidth="1"/>
+    <col min="10" max="11" width="10.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="52" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="6" customFormat="1" ht="45" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="4"/>
+    <row r="4" spans="1:12" ht="15" customHeight="1">
+      <c r="G4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="4">
+        <f>5/(Avogadro_constant*Cell_volume)</f>
+        <v>3.0761658668635413E-7</v>
+      </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="4"/>
+    <row r="5" spans="1:12" ht="15" customHeight="1">
+      <c r="G5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="4">
+        <f>100/(Avogadro_constant*Cell_volume)</f>
+        <v>6.1523317337270823E-6</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+    <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" customHeight="1">
+      <c r="B12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:9" ht="15" customHeight="1">
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9" ht="15" customHeight="1">
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:9" ht="15" customHeight="1">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:9" ht="15" customHeight="1">
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:9" ht="15" customHeight="1">
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:9" ht="15" customHeight="1">
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:9" ht="15" customHeight="1">
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:9" ht="15" customHeight="1">
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:9" ht="15" customHeight="1">
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:9" ht="15" customHeight="1">
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:9" ht="15" customHeight="1">
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:9" ht="15" customHeight="1">
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:9" ht="15" customHeight="1">
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:9" ht="15" customHeight="1">
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:9" ht="15" customHeight="1">
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:9" ht="15" customHeight="1">
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:9" ht="15" customHeight="1">
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:9" ht="15" customHeight="1">
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:9" ht="15" customHeight="1">
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:9" ht="15" customHeight="1">
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:9" ht="15" customHeight="1">
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:9" ht="15" customHeight="1">
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:9" ht="15" customHeight="1">
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:9" ht="15" customHeight="1">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:9" ht="15" customHeight="1">
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:9" ht="15" customHeight="1">
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:9" ht="15" customHeight="1">
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:9" ht="15" customHeight="1">
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:9" ht="15" customHeight="1">
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:9" ht="15" customHeight="1">
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:9" ht="15" customHeight="1">
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:9" ht="15" customHeight="1">
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:9" ht="15" customHeight="1">
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:9" ht="15" customHeight="1">
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
     </row>
-    <row r="51" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:9" ht="15" customHeight="1">
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:9" ht="15" customHeight="1">
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
     </row>
-    <row r="53" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:9" ht="15" customHeight="1">
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
     </row>
-    <row r="54" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:9" ht="15" customHeight="1">
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
     </row>
-    <row r="55" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:9" ht="15" customHeight="1">
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
     </row>
-    <row r="56" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:9" ht="15" customHeight="1">
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
     </row>
-    <row r="57" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:9" ht="15" customHeight="1">
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
     </row>
-    <row r="58" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:9" ht="15" customHeight="1">
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
     </row>
-    <row r="59" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:9" ht="15" customHeight="1">
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:9" ht="15" customHeight="1">
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:9" ht="15" customHeight="1">
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
-    <row r="62" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:9" ht="15" customHeight="1">
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
-    <row r="63" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:9" ht="15" customHeight="1">
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
-    <row r="64" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:9" ht="15" customHeight="1">
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
-    <row r="65" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:9" ht="15" customHeight="1">
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
-    <row r="66" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:9" ht="15" customHeight="1">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="67" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:9" ht="15" customHeight="1">
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:9" ht="15" customHeight="1">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="69" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:9" ht="15" customHeight="1">
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
-    <row r="70" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:9" ht="15" customHeight="1">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="71" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:9" ht="15" customHeight="1">
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
-    <row r="72" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:9" ht="15" customHeight="1">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="73" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:9" ht="15" customHeight="1">
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:9" ht="15" customHeight="1">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="75" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:9" ht="15" customHeight="1">
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
-    <row r="76" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:9" ht="15" customHeight="1">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:9" ht="15" customHeight="1">
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
-    <row r="78" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:9" ht="15" customHeight="1">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="79" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:9" ht="15" customHeight="1">
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
-    <row r="80" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:9" ht="15" customHeight="1">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="81" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:9" ht="15" customHeight="1">
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
-    <row r="82" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:9" ht="15" customHeight="1">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="83" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:9" ht="15" customHeight="1">
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
-    <row r="84" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:9" ht="15" customHeight="1">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:9" ht="15" customHeight="1">
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
     </row>
-    <row r="86" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:9" ht="15" customHeight="1">
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="87" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:9" ht="15" customHeight="1">
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
-    <row r="88" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:9" ht="15" customHeight="1">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:9" ht="15" customHeight="1">
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:9" ht="15" customHeight="1">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:9" ht="15" customHeight="1">
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:9" ht="15" customHeight="1">
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:9" ht="15" customHeight="1">
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:9" ht="15" customHeight="1">
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:9" ht="15" customHeight="1">
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:9" ht="15" customHeight="1">
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:9" ht="15" customHeight="1">
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:9" ht="15" customHeight="1">
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:9" ht="15" customHeight="1">
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:9" ht="15" customHeight="1">
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:9" ht="15" customHeight="1">
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:9" ht="15" customHeight="1">
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:9" ht="15" customHeight="1">
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:9" ht="15" customHeight="1">
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:9" ht="15" customHeight="1">
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:9" ht="15" customHeight="1">
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:9" ht="15" customHeight="1">
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:9" ht="15" customHeight="1">
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:9" ht="15" customHeight="1">
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:9" ht="15" customHeight="1">
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:9" ht="15" customHeight="1">
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:9" ht="15" customHeight="1">
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:9" ht="15" customHeight="1">
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:9" ht="15" customHeight="1">
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
     </row>
-    <row r="115" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:9" ht="15" customHeight="1">
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:9" ht="15" customHeight="1">
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:9" ht="15" customHeight="1">
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
     </row>
-    <row r="118" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:9" ht="15" customHeight="1">
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
     </row>
-    <row r="119" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:9" ht="15" customHeight="1">
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
     </row>
-    <row r="120" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:9" ht="15" customHeight="1">
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:9" ht="15" customHeight="1">
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
     </row>
-    <row r="122" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:9" ht="15" customHeight="1">
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
     </row>
-    <row r="123" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:9" ht="15" customHeight="1">
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:9" ht="15" customHeight="1">
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
     </row>
-    <row r="125" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:9" ht="15" customHeight="1">
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
     </row>
-    <row r="126" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:9" ht="15" customHeight="1">
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
     </row>
-    <row r="127" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:9" ht="15" customHeight="1">
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
     </row>
-    <row r="128" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:9" ht="15" customHeight="1">
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
     </row>
-    <row r="129" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:9" ht="15" customHeight="1">
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
     </row>
-    <row r="130" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:9" ht="15" customHeight="1">
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
     </row>
-    <row r="131" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:9" ht="15" customHeight="1">
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
     </row>
-    <row r="132" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:9" ht="15" customHeight="1">
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
     </row>
-    <row r="133" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:9" ht="15" customHeight="1">
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
     </row>
-    <row r="134" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:9" ht="15" customHeight="1">
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
     </row>
-    <row r="135" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:9" ht="15" customHeight="1">
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
     </row>
-    <row r="136" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:9" ht="15" customHeight="1">
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
     </row>
-    <row r="137" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:9" ht="15" customHeight="1">
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
     </row>
-    <row r="138" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:9" ht="15" customHeight="1">
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
     </row>
-    <row r="139" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:9" ht="15" customHeight="1">
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:9" ht="15" customHeight="1">
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
     </row>
-    <row r="141" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:9" ht="15" customHeight="1">
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
     </row>
-    <row r="142" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:9" ht="15" customHeight="1">
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
     </row>
-    <row r="143" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:9" ht="15" customHeight="1">
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
     </row>
-    <row r="144" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:9" ht="15" customHeight="1">
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
     </row>
-    <row r="145" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="8:9" ht="15" customHeight="1">
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
     </row>
-    <row r="146" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:9" ht="15" customHeight="1">
       <c r="H146" s="4"/>
+      <c r="I146" s="4"/>
+    </row>
+    <row r="147" spans="8:9" ht="15" customHeight="1">
+      <c r="H147" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L147"/>
+  <autoFilter ref="A2:L148"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1626,22 +1780,22 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="3" customWidth="1"/>
     <col min="5" max="5" width="14" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="28.28515625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="6" width="18.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="45" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1676,444 +1830,449 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1">
       <c r="G2" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="G5" s="7"/>
     </row>
-    <row r="26" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:7" ht="15" customHeight="1">
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:7" ht="15" customHeight="1">
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:7" ht="15" customHeight="1">
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:7" ht="15" customHeight="1">
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:7" ht="15" customHeight="1">
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:7" ht="15" customHeight="1">
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:7" ht="15" customHeight="1">
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" ht="15" customHeight="1">
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" ht="15" customHeight="1">
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" ht="15" customHeight="1">
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" ht="15" customHeight="1">
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" ht="15" customHeight="1">
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" ht="15" customHeight="1">
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:7" ht="15" customHeight="1">
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:7" ht="15" customHeight="1">
       <c r="G40" s="7"/>
     </row>
-    <row r="42" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:7" ht="15" customHeight="1">
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:7" ht="15" customHeight="1">
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:7" ht="15" customHeight="1">
       <c r="G44" s="7"/>
     </row>
-    <row r="46" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:7" ht="15" customHeight="1">
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:7" ht="15" customHeight="1">
       <c r="G47" s="7"/>
     </row>
-    <row r="52" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:7" ht="15" customHeight="1">
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:7" ht="15" customHeight="1">
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:7" ht="15" customHeight="1">
       <c r="G54" s="7"/>
     </row>
-    <row r="87" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:8" ht="15" customHeight="1">
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:8" ht="15" customHeight="1">
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:8" ht="15" customHeight="1">
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:8" ht="15" customHeight="1">
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:8" ht="15" customHeight="1">
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
     </row>
-    <row r="92" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:8" ht="15" customHeight="1">
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:8" ht="15" customHeight="1">
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
     </row>
-    <row r="94" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:8" ht="15" customHeight="1">
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
-    <row r="95" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:8" ht="15" customHeight="1">
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
     </row>
-    <row r="96" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="7:8" ht="15" customHeight="1">
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
     </row>
-    <row r="97" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="7:8" ht="15" customHeight="1">
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
     </row>
-    <row r="98" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="7:8" ht="15" customHeight="1">
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
     </row>
-    <row r="99" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="7:8" ht="15" customHeight="1">
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
     </row>
-    <row r="100" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="7:8" ht="15" customHeight="1">
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
     </row>
-    <row r="101" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="7:8" ht="15" customHeight="1">
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
     </row>
-    <row r="102" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="7:8" ht="15" customHeight="1">
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
     </row>
-    <row r="103" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="7:8" ht="15" customHeight="1">
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
     </row>
-    <row r="104" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="7:8" ht="15" customHeight="1">
       <c r="G104" s="7"/>
       <c r="H104" s="7"/>
     </row>
-    <row r="105" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="7:8" ht="15" customHeight="1">
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
     </row>
-    <row r="106" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="7:8" ht="15" customHeight="1">
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
     </row>
-    <row r="107" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="7:8" ht="15" customHeight="1">
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
     </row>
-    <row r="108" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="7:8" ht="15" customHeight="1">
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
     </row>
-    <row r="109" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="7:8" ht="15" customHeight="1">
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
     </row>
-    <row r="110" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="7:8" ht="15" customHeight="1">
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
     </row>
-    <row r="111" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="7:8" ht="15" customHeight="1">
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
     </row>
-    <row r="112" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="7:8" ht="15" customHeight="1">
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
     </row>
-    <row r="113" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="7:8" ht="15" customHeight="1">
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
     </row>
-    <row r="114" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="7:8" ht="15" customHeight="1">
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
     </row>
-    <row r="115" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="7:8" ht="15" customHeight="1">
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
     </row>
-    <row r="116" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="7:8" ht="15" customHeight="1">
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
     </row>
-    <row r="117" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="7:8" ht="15" customHeight="1">
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
     </row>
-    <row r="118" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="7:8" ht="15" customHeight="1">
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
     </row>
-    <row r="119" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="7:8" ht="15" customHeight="1">
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
     </row>
-    <row r="120" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="7:8" ht="15" customHeight="1">
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
     </row>
-    <row r="121" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:8" ht="15" customHeight="1">
       <c r="G121" s="7"/>
       <c r="H121" s="7"/>
     </row>
-    <row r="122" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="7:8" ht="15" customHeight="1">
       <c r="G122" s="7"/>
       <c r="H122" s="7"/>
     </row>
-    <row r="123" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="7:8" ht="15" customHeight="1">
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
     </row>
-    <row r="124" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="7:8" ht="15" customHeight="1">
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
     </row>
-    <row r="125" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="7:8" ht="15" customHeight="1">
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
     </row>
-    <row r="126" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="7:8" ht="15" customHeight="1">
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
     </row>
-    <row r="127" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="7:8" ht="15" customHeight="1">
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
     </row>
-    <row r="128" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="7:8" ht="15" customHeight="1">
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
     </row>
-    <row r="129" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:8" ht="15" customHeight="1">
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
     </row>
-    <row r="130" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="7:8" ht="15" customHeight="1">
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
     </row>
-    <row r="131" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="7:8" ht="15" customHeight="1">
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
     </row>
-    <row r="132" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="7:8" ht="15" customHeight="1">
       <c r="G132" s="7"/>
       <c r="H132" s="7"/>
     </row>
-    <row r="133" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="7:8" ht="15" customHeight="1">
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
     </row>
-    <row r="134" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="7:8" ht="15" customHeight="1">
       <c r="G134" s="7"/>
       <c r="H134" s="7"/>
     </row>
-    <row r="135" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="7:8" ht="15" customHeight="1">
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
     </row>
-    <row r="136" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="7:8" ht="15" customHeight="1">
       <c r="G136" s="7"/>
       <c r="H136" s="7"/>
     </row>
-    <row r="137" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="7:8" ht="15" customHeight="1">
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
     </row>
-    <row r="138" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="7:8" ht="15" customHeight="1">
       <c r="G138" s="7"/>
       <c r="H138" s="7"/>
     </row>
-    <row r="139" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="7:8" ht="15" customHeight="1">
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
     </row>
-    <row r="140" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="7:8" ht="15" customHeight="1">
       <c r="G140" s="7"/>
       <c r="H140" s="7"/>
     </row>
-    <row r="141" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="7:8" ht="15" customHeight="1">
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
     </row>
-    <row r="142" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="7:8" ht="15" customHeight="1">
       <c r="G142" s="7"/>
       <c r="H142" s="7"/>
     </row>
-    <row r="143" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="7:8" ht="15" customHeight="1">
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
     </row>
-    <row r="144" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="7:8" ht="15" customHeight="1">
       <c r="G144" s="7"/>
       <c r="H144" s="7"/>
     </row>
-    <row r="145" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="7:8" ht="15" customHeight="1">
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
     </row>
-    <row r="146" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="7:8" ht="15" customHeight="1">
       <c r="G146" s="7"/>
       <c r="H146" s="7"/>
     </row>
-    <row r="147" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="7:8" ht="15" customHeight="1">
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
     </row>
-    <row r="148" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="7:8" ht="15" customHeight="1">
       <c r="G148" s="7"/>
       <c r="H148" s="7"/>
     </row>
-    <row r="149" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="7:8" ht="15" customHeight="1">
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
     </row>
-    <row r="150" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="7:8" ht="15" customHeight="1">
       <c r="G150" s="7"/>
       <c r="H150" s="7"/>
     </row>
-    <row r="151" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="7:8" ht="15" customHeight="1">
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
     </row>
-    <row r="152" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="7:8" ht="15" customHeight="1">
       <c r="G152" s="7"/>
       <c r="H152" s="7"/>
     </row>
-    <row r="153" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="7:8" ht="15" customHeight="1">
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
     </row>
-    <row r="154" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="7:8" ht="15" customHeight="1">
       <c r="G154" s="7"/>
       <c r="H154" s="7"/>
     </row>
-    <row r="155" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="7:8" ht="15" customHeight="1">
       <c r="G155" s="7"/>
       <c r="H155" s="7"/>
     </row>
-    <row r="156" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="7:8" ht="15" customHeight="1">
       <c r="G156" s="7"/>
       <c r="H156" s="7"/>
     </row>
-    <row r="157" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="7:8" ht="15" customHeight="1">
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
     </row>
-    <row r="158" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="7:8" ht="15" customHeight="1">
       <c r="G158" s="7"/>
       <c r="H158" s="7"/>
     </row>
-    <row r="159" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="7:8" ht="15" customHeight="1">
       <c r="G159" s="7"/>
       <c r="H159" s="7"/>
     </row>
-    <row r="160" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="7:8" ht="15" customHeight="1">
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
     </row>
-    <row r="161" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:8" ht="15" customHeight="1">
       <c r="G161" s="7"/>
       <c r="H161" s="7"/>
     </row>
-    <row r="162" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="7:8" ht="15" customHeight="1">
       <c r="G162" s="7"/>
       <c r="H162" s="7"/>
     </row>
-    <row r="163" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="7:8" ht="15" customHeight="1">
       <c r="G163" s="7"/>
       <c r="H163" s="7"/>
     </row>
-    <row r="164" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="7:8" ht="15" customHeight="1">
       <c r="G164" s="7"/>
       <c r="H164" s="7"/>
     </row>
-    <row r="165" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="7:8" ht="15" customHeight="1">
       <c r="G165" s="7"/>
       <c r="H165" s="7"/>
     </row>
-    <row r="166" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="7:8" ht="15" customHeight="1">
       <c r="G166" s="7"/>
       <c r="H166" s="7"/>
     </row>
-    <row r="167" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="7:8" ht="15" customHeight="1">
       <c r="G167" s="7"/>
       <c r="H167" s="7"/>
     </row>
-    <row r="168" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="7:8" ht="15" customHeight="1">
       <c r="G168" s="7"/>
       <c r="H168" s="7"/>
     </row>
-    <row r="169" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="7:8" ht="15" customHeight="1">
       <c r="G169" s="7"/>
       <c r="H169" s="7"/>
     </row>
-    <row r="170" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="7:8" ht="15" customHeight="1">
       <c r="G170" s="7"/>
       <c r="H170" s="7"/>
     </row>
-    <row r="171" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="7:8" ht="15" customHeight="1">
       <c r="G171" s="7"/>
       <c r="H171" s="7"/>
     </row>
-    <row r="172" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="7:8" ht="15" customHeight="1">
       <c r="G172" s="7"/>
       <c r="H172" s="7"/>
     </row>
-    <row r="173" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="7:8" ht="15" customHeight="1">
       <c r="G173" s="7"/>
       <c r="H173" s="7"/>
     </row>
-    <row r="174" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="7:8" ht="15" customHeight="1">
       <c r="G174" s="7"/>
       <c r="H174" s="7"/>
     </row>
-    <row r="175" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="7:8" ht="15" customHeight="1">
       <c r="G175" s="7"/>
       <c r="H175" s="7"/>
     </row>
-    <row r="176" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="7:8" ht="15" customHeight="1">
       <c r="G176" s="7"/>
       <c r="H176" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K177"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2121,25 +2280,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD8"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="12">
       <c r="A1" s="1" t="str">
         <f>Submodels!$A$1</f>
         <v>ID</v>
@@ -2160,7 +2319,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="12">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -2173,8 +2332,11 @@
       <c r="E2" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2350,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="48">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -2208,7 +2370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -2228,7 +2390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -2248,6 +2410,11 @@
   </sheetData>
   <autoFilter ref="A1:F6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2262,16 +2429,16 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2288,7 +2455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -2302,7 +2469,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -2316,7 +2483,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -2333,7 +2500,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -2347,7 +2514,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
@@ -2361,7 +2528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
@@ -2375,7 +2542,7 @@
         <v>815332823</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -2389,7 +2556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>74</v>
       </c>
@@ -2403,7 +2570,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -2417,7 +2584,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -2431,7 +2598,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>83</v>
       </c>
@@ -2445,7 +2612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>86</v>
       </c>
@@ -2459,7 +2626,7 @@
         <v>33184</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>89</v>
       </c>
@@ -2473,7 +2640,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>90</v>
       </c>
@@ -2487,7 +2654,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>91</v>
       </c>
@@ -2501,7 +2668,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>92</v>
       </c>
@@ -2515,7 +2682,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>93</v>
       </c>
@@ -2529,7 +2696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>94</v>
       </c>
@@ -2543,7 +2710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
@@ -2560,5 +2727,65 @@
   </sheetData>
   <autoFilter ref="A1:E20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="10">
+        <v>6.02E+23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3">
+        <f>(0.3^3)*1000/1000000000000000000</f>
+        <v>2.7000000000000001E-17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>